<commit_message>
find and update excel cell value
</commit_message>
<xml_diff>
--- a/tournament/points_table.xlsx
+++ b/tournament/points_table.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\2nd Trimester\CM1601 [PRO] Programming Fundamentals\CW\coursework\tournament\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{8D65E0DC-6092-4518-8C70-E00F4513AB61}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowHeight="9017" windowWidth="16663" xWindow="-103" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="343"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Group A</t>
   </si>
@@ -71,13 +77,17 @@
   </si>
   <si>
     <t>Sunrisers_SriLanka</t>
+  </si>
+  <si>
+    <t>88</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,19 +137,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -148,10 +166,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -186,7 +204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,9 +236,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,6 +288,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -307,7 +361,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -316,13 +370,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -332,7 +386,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -341,7 +395,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -350,7 +404,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -360,12 +414,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -396,7 +450,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -415,7 +469,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -427,14 +481,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,12 +525,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="n">
+        <v>89.0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -504,7 +560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -539,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -574,7 +630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -610,6 +666,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>